<commit_message>
add capability to run full integration tests
</commit_message>
<xml_diff>
--- a/src/XlsToEf.Tests/TestExcelDoc.xlsx
+++ b/src/XlsToEf.Tests/TestExcelDoc.xlsx
@@ -25,12 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Price</t>
+    <t>Cat</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>Persian</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Main Coon</t>
+  </si>
+  <si>
+    <t>Tabby</t>
   </si>
 </sst>
 </file>
@@ -394,20 +403,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
-        <v>11</v>
+      <c r="B1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -415,7 +427,23 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>15</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>